<commit_message>
tippmix integrated to ML_PL_new
</commit_message>
<xml_diff>
--- a/ML_PL_new/fuzz_teams.xlsx
+++ b/ML_PL_new/fuzz_teams.xlsx
@@ -4333,7 +4333,11 @@
           <t>Rio Ave FC</t>
         </is>
       </c>
-      <c r="E112" t="inlineStr"/>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Rio Ave</t>
+        </is>
+      </c>
       <c r="F112" t="inlineStr">
         <is>
           <t>Vila do Conde</t>
@@ -4498,7 +4502,11 @@
           <t>Ajax</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr"/>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Ajax</t>
+        </is>
+      </c>
       <c r="F117" t="inlineStr">
         <is>
           <t>Amsterdam</t>

</xml_diff>

<commit_message>
tippmix isolated from main file, moved to ML_PL_new
</commit_message>
<xml_diff>
--- a/ML_PL_new/fuzz_teams.xlsx
+++ b/ML_PL_new/fuzz_teams.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="387">
   <si>
     <t>Country</t>
   </si>
@@ -1171,6 +1171,15 @@
   </si>
   <si>
     <t>AVS SAD</t>
+  </si>
+  <si>
+    <t>Nacional Madeira</t>
+  </si>
+  <si>
+    <t>F. Sittard</t>
+  </si>
+  <si>
+    <t>PSV</t>
   </si>
 </sst>
 </file>
@@ -1537,12 +1546,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1927,6 +1937,9 @@
       <c r="D17" t="s">
         <v>53</v>
       </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
       <c r="F17" t="s">
         <v>54</v>
       </c>
@@ -1947,6 +1960,9 @@
       <c r="D18" t="s">
         <v>56</v>
       </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
       <c r="F18" t="s">
         <v>56</v>
       </c>
@@ -3600,6 +3616,9 @@
       <c r="D90" t="s">
         <v>203</v>
       </c>
+      <c r="E90" t="s">
+        <v>203</v>
+      </c>
       <c r="F90" t="s">
         <v>203</v>
       </c>
@@ -3643,6 +3662,9 @@
       <c r="D92" t="s">
         <v>207</v>
       </c>
+      <c r="E92" t="s">
+        <v>205</v>
+      </c>
       <c r="F92" t="s">
         <v>208</v>
       </c>
@@ -3847,6 +3869,9 @@
       <c r="D101" t="s">
         <v>230</v>
       </c>
+      <c r="E101" t="s">
+        <v>229</v>
+      </c>
       <c r="F101" t="s">
         <v>227</v>
       </c>
@@ -3867,6 +3892,9 @@
       <c r="D102" t="s">
         <v>232</v>
       </c>
+      <c r="E102" t="s">
+        <v>232</v>
+      </c>
       <c r="F102" t="s">
         <v>227</v>
       </c>
@@ -3887,6 +3915,9 @@
       <c r="D103" t="s">
         <v>234</v>
       </c>
+      <c r="E103" t="s">
+        <v>234</v>
+      </c>
       <c r="F103" t="s">
         <v>234</v>
       </c>
@@ -3930,6 +3961,9 @@
       <c r="D105" t="s">
         <v>240</v>
       </c>
+      <c r="E105" t="s">
+        <v>239</v>
+      </c>
       <c r="F105" t="s">
         <v>241</v>
       </c>
@@ -3973,6 +4007,9 @@
       <c r="D107" t="s">
         <v>247</v>
       </c>
+      <c r="E107" t="s">
+        <v>247</v>
+      </c>
       <c r="F107" t="s">
         <v>247</v>
       </c>
@@ -3993,6 +4030,9 @@
       <c r="D108" t="s">
         <v>252</v>
       </c>
+      <c r="E108" t="s">
+        <v>250</v>
+      </c>
       <c r="F108" t="s">
         <v>253</v>
       </c>
@@ -4036,6 +4076,9 @@
       <c r="D110" t="s">
         <v>259</v>
       </c>
+      <c r="E110" t="s">
+        <v>384</v>
+      </c>
       <c r="F110" t="s">
         <v>260</v>
       </c>
@@ -4056,6 +4099,9 @@
       <c r="D111" t="s">
         <v>263</v>
       </c>
+      <c r="E111" t="s">
+        <v>262</v>
+      </c>
       <c r="F111" t="s">
         <v>262</v>
       </c>
@@ -4099,6 +4145,9 @@
       <c r="D113" t="s">
         <v>269</v>
       </c>
+      <c r="E113" t="s">
+        <v>269</v>
+      </c>
       <c r="F113" t="s">
         <v>270</v>
       </c>
@@ -4142,6 +4191,9 @@
       <c r="D115" t="s">
         <v>277</v>
       </c>
+      <c r="E115" t="s">
+        <v>276</v>
+      </c>
       <c r="F115" t="s">
         <v>227</v>
       </c>
@@ -4208,6 +4260,9 @@
       <c r="D118" t="s">
         <v>286</v>
       </c>
+      <c r="E118" t="s">
+        <v>286</v>
+      </c>
       <c r="F118" t="s">
         <v>287</v>
       </c>
@@ -4228,6 +4283,9 @@
       <c r="D119" t="s">
         <v>289</v>
       </c>
+      <c r="E119" t="s">
+        <v>289</v>
+      </c>
       <c r="F119" t="s">
         <v>290</v>
       </c>
@@ -4248,6 +4306,9 @@
       <c r="D120" t="s">
         <v>293</v>
       </c>
+      <c r="E120" t="s">
+        <v>385</v>
+      </c>
       <c r="F120" t="s">
         <v>294</v>
       </c>
@@ -4268,6 +4329,9 @@
       <c r="D121" t="s">
         <v>296</v>
       </c>
+      <c r="E121" t="s">
+        <v>296</v>
+      </c>
       <c r="F121" t="s">
         <v>298</v>
       </c>
@@ -4311,6 +4375,9 @@
       <c r="D123" t="s">
         <v>302</v>
       </c>
+      <c r="E123" t="s">
+        <v>302</v>
+      </c>
       <c r="F123" t="s">
         <v>302</v>
       </c>
@@ -4354,6 +4421,9 @@
       <c r="D125" t="s">
         <v>308</v>
       </c>
+      <c r="E125" t="s">
+        <v>308</v>
+      </c>
       <c r="F125" t="s">
         <v>309</v>
       </c>
@@ -4374,6 +4444,9 @@
       <c r="D126" t="s">
         <v>312</v>
       </c>
+      <c r="E126" t="s">
+        <v>311</v>
+      </c>
       <c r="F126" t="s">
         <v>311</v>
       </c>
@@ -4394,6 +4467,9 @@
       <c r="D127" t="s">
         <v>314</v>
       </c>
+      <c r="E127" t="s">
+        <v>386</v>
+      </c>
       <c r="F127" t="s">
         <v>315</v>
       </c>
@@ -4414,6 +4490,9 @@
       <c r="D128" t="s">
         <v>317</v>
       </c>
+      <c r="E128" t="s">
+        <v>317</v>
+      </c>
       <c r="F128" t="s">
         <v>290</v>
       </c>
@@ -4478,6 +4557,9 @@
         <v>328</v>
       </c>
       <c r="D131" t="s">
+        <v>328</v>
+      </c>
+      <c r="E131" t="s">
         <v>328</v>
       </c>
       <c r="F131" t="s">

</xml_diff>